<commit_message>
daily service report location added
</commit_message>
<xml_diff>
--- a/tmp/dailyReport.xlsx
+++ b/tmp/dailyReport.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1E8AE6-AD18-4AA5-9E36-846C955DD7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FFD349-6AA6-46DF-AD6D-11BCAFCC8CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,15 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Service Type</t>
-  </si>
-  <si>
-    <t>Technician Comment</t>
-  </si>
-  <si>
-    <t>Technician Name</t>
   </si>
   <si>
     <t>Image 1</t>
@@ -61,6 +55,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Operator Comment</t>
+  </si>
+  <si>
+    <t>Operator Name</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -153,11 +156,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -172,11 +224,27 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -206,7 +274,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:colOff>847725</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
@@ -237,8 +305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1409700" y="104775"/>
-          <a:ext cx="3533775" cy="1085850"/>
+          <a:off x="1181100" y="104775"/>
+          <a:ext cx="4371975" cy="1085850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -572,93 +640,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21" style="13" customWidth="1"/>
+    <col min="4" max="4" width="23" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+    <row r="1" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+    <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>